<commit_message>
ppPlot y organizar doc Funciones Aux
</commit_message>
<xml_diff>
--- a/Avances paquete.xlsx
+++ b/Avances paquete.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epnecuador-my.sharepoint.com/personal/andrea_barahona_epn_edu_ec/Documents/PasantiasUDC/Libro_TidyQualityTools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{1F8B6C19-C86C-41D0-B0BC-8FFE12B9195D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{525B2045-45A4-4F1A-8D35-F1911364C194}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="8_{1F8B6C19-C86C-41D0-B0BC-8FFE12B9195D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{587ED6E3-4A13-44FE-8F01-AE50B16D998E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C95EA655-6F4D-4D28-BCDA-105F80DE6639}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C95EA655-6F4D-4D28-BCDA-105F80DE6639}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Avances" sheetId="1" r:id="rId1"/>
     <sheet name="Funciones que ya están" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -531,37 +531,37 @@
     <t>.charToDistFunc</t>
   </si>
   <si>
-    <t>.confintbeta</t>
-  </si>
-  <si>
-    <t>.confincauchy</t>
-  </si>
-  <si>
-    <t>.confintexp</t>
-  </si>
-  <si>
-    <t>.confintlnorm</t>
-  </si>
-  <si>
-    <t>.confintlogis</t>
-  </si>
-  <si>
-    <t>.confintnorm</t>
-  </si>
-  <si>
-    <t>.confintweibull</t>
-  </si>
-  <si>
-    <t>.gamma3</t>
-  </si>
-  <si>
-    <t>.lognormal3</t>
-  </si>
-  <si>
-    <t>.weibull3</t>
-  </si>
-  <si>
     <t>Funcion distribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 .confincauchy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 .confintexp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 .confintlnorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 .confintnorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 .confintlogis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 .confintweibull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 .gamma3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 .lognormal3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 .weibull3</t>
+  </si>
+  <si>
+    <t>internals.r : .confintbeta</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -608,12 +608,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,7 +720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -734,9 +728,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -749,6 +740,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1089,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A3DCFC-D9FB-48AC-8632-C7F2B78E3A7E}">
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92:XFD97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1960,7 +1953,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="10" t="s">
+      <c r="A96" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B96" s="4" t="s">
@@ -1974,7 +1967,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="8" t="s">
         <v>98</v>
       </c>
       <c r="B97" s="4" t="s">
@@ -1988,17 +1981,17 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="7" t="s">
+      <c r="A98" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="B98" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C98" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="D98" s="9">
-        <v>45426</v>
+      <c r="C98" s="5">
+        <v>1</v>
+      </c>
+      <c r="D98" s="6">
+        <v>45427</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -2326,16 +2319,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA47FEC-19D0-4F0E-91D4-562668967302}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.44140625" customWidth="1"/>
-    <col min="2" max="2" width="64.5546875" customWidth="1"/>
+    <col min="2" max="2" width="38.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -2347,212 +2341,239 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>150</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
-      <c r="B4" s="17" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="14" t="s">
         <v>152</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="17" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="14" t="s">
         <v>151</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="15" t="s">
         <v>153</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="13" t="s">
         <v>139</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="14" t="s">
         <v>140</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-      <c r="B9" s="17" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="14" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="17"/>
+      <c r="B19" s="20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="17"/>
+      <c r="B20" s="20" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="17"/>
+      <c r="B21" s="20" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="17"/>
+      <c r="B23" s="20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="17"/>
+      <c r="B24" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="17"/>
+      <c r="B25" s="20" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="17"/>
+      <c r="B26" s="20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="17"/>
+      <c r="B27" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="17"/>
+      <c r="B28" s="20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="17"/>
+      <c r="B29" s="20" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" s="17" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="17"/>
+      <c r="B30" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
-      <c r="B13" s="18" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="17"/>
+      <c r="B31" s="20" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="17" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="17" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" s="17" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="17" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" s="17" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="17" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="17" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="17" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
-      <c r="B25" s="17" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
-      <c r="B26" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
-      <c r="B28" s="17" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="20"/>
-      <c r="B29" s="17" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="20"/>
-      <c r="B30" s="17" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="21"/>
-      <c r="B31" s="18" t="s">
-        <v>173</v>
-      </c>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="17"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="17"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="17"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="17"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="17"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="18"/>
+      <c r="B39" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>